<commit_message>
Added class motto + added 5 ninja skills in the documentation.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Ninja/Documentation/NinjaSkills.xlsx
+++ b/GameDesign/Class/Ninja/Documentation/NinjaSkills.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\Ninja\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
+    <sheet name="1-Cyanide" sheetId="1" r:id="rId1"/>
+    <sheet name="2-Geta" sheetId="2" r:id="rId2"/>
+    <sheet name="3-Jika-Tabi" sheetId="3" r:id="rId3"/>
+    <sheet name="4-Ninjato" sheetId="4" r:id="rId4"/>
+    <sheet name="5-Kunai" sheetId="5" r:id="rId5"/>
+    <sheet name="6-Shuriken" sheetId="6" r:id="rId6"/>
     <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="72">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -90,6 +90,165 @@
   </si>
   <si>
     <t>[[Number of turns between two casts: -  ]]</t>
+  </si>
+  <si>
+    <t>Cyanide</t>
+  </si>
+  <si>
+    <t>[[Range: 0 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: No ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Cyanide''.</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell]]</t>
+  </si>
+  <si>
+    <t>[[AP: 1 ]]</t>
+  </si>
+  <si>
+    <t>Damages: 10 dark per lvl of effect.</t>
+  </si>
+  <si>
+    <t>[[Cyanide]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Geta</t>
+  </si>
+  <si>
+    <t>My sharp weapons got a surprise for you...</t>
+  </si>
+  <si>
+    <t>Effect name: ''Geta''.</t>
+  </si>
+  <si>
+    <t>When walking over glyph or trap, dosn't activate them.</t>
+  </si>
+  <si>
+    <t>[[AP: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0-1 ]]</t>
+  </si>
+  <si>
+    <t>[[Geta]] (1 turn)</t>
+  </si>
+  <si>
+    <t>You thought such trap would restraint me ? How silly.</t>
+  </si>
+  <si>
+    <t>Jika-Tabi</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 3 ]]</t>
+  </si>
+  <si>
+    <t>Self targeting: [[Boost MP by 4]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Ally targeting: [[Boost MP by 2]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Jika-Tabi''.</t>
+  </si>
+  <si>
+    <t>My speed is beyond your limit</t>
+  </si>
+  <si>
+    <t>Ninjato</t>
+  </si>
+  <si>
+    <t>[[AP: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  50-60 earth ]]</t>
+  </si>
+  <si>
+    <t>I stop hiding, let's face me!</t>
+  </si>
+  <si>
+    <t>Kunai</t>
+  </si>
+  <si>
+    <t>[[Range: 2-5 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: No ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  30-35 air ]]</t>
+  </si>
+  <si>
+    <t>If under ''Cyanide'' effect: [[Poison +1 lvl on target]] (2 turns)</t>
+  </si>
+  <si>
+    <t>If under ''Cyanide'' effect: [[Poison +2 lvls on target]] (2 turns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A simple and effective solution to eliminate an annoying </t>
+  </si>
+  <si>
+    <t>opponent while remaining in the obscurity.</t>
+  </si>
+  <si>
+    <t>Shuriken</t>
+  </si>
+  <si>
+    <t>[[Range: 2-4 ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Distracted''.</t>
+  </si>
+  <si>
+    <t>[[Damage:  10-15 air ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Reduce target power by 100]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Reduce target resistance by 15%]] (2 turns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At first sight, my shuriken seem weak, </t>
+  </si>
+  <si>
+    <t>they true power hide in they side effect.</t>
   </si>
 </sst>
 </file>
@@ -129,7 +288,7 @@
       <family val="5"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -200,6 +365,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +703,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -549,40 +715,38 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -594,134 +758,82 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -948,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +1083,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -983,66 +1095,64 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1054,45 +1164,37 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1103,59 +1205,22 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1165,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1253,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1200,66 +1265,64 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1271,108 +1334,63 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1382,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1423,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1417,40 +1435,38 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1462,71 +1478,63 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1537,59 +1545,13 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="10"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1599,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1584,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1634,14 +1596,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1653,7 +1615,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1667,7 +1629,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1679,21 +1641,21 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1705,14 +1667,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1724,26 +1686,26 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1752,61 +1714,33 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1816,10 +1750,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1773,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1851,14 +1785,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1870,160 +1804,141 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="1"/>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
+      <c r="C29" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a skill in Ninja doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Ninja/Documentation/NinjaSkills.xlsx
+++ b/GameDesign/Class/Ninja/Documentation/NinjaSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1-Cyanide" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="4-Ninjato" sheetId="4" r:id="rId4"/>
     <sheet name="5-Kunai" sheetId="5" r:id="rId5"/>
     <sheet name="6-Shuriken" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
+    <sheet name="7-Makibishi" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
     <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -249,6 +249,36 @@
   </si>
   <si>
     <t>they true power hide in they side effect.</t>
+  </si>
+  <si>
+    <t>Makibishi</t>
+  </si>
+  <si>
+    <t>[[Line of sight: No ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 5 ]]</t>
+  </si>
+  <si>
+    <t>*The poison effect is there if the spell was used whit ''Cyanide''. Even if the player don't have ''Cyanide'' the other turn, the poison is applyed.                                                                                                          *If the player used this spell whitout ''Cyanide'', the spell will not apply poison, even if the player as the ''Cyanide'' effect.</t>
+  </si>
+  <si>
+    <t>Glyph (3 turns)</t>
+  </si>
+  <si>
+    <t>[[Damage:  25 earth ]]</t>
+  </si>
+  <si>
+    <t>If under ''Cyanide'' effect: [[Poison +1 lvl on target ]] (2 turns)</t>
+  </si>
+  <si>
+    <t>The damage are triggered at the start of a target turn on the area and for each of its moving into a makibishi cell.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Circle of 4 cell radius ]] (60% rate per cell in area)</t>
+  </si>
+  <si>
+    <t>Let see if you're brave enough to follow me around these.</t>
   </si>
 </sst>
 </file>
@@ -320,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -337,11 +367,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -366,6 +405,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1403,7 +1448,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,10 +1993,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,7 +2016,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1983,66 +2028,64 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2054,108 +2097,77 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="98.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ninja skills documentation DONE!
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Ninja/Documentation/NinjaSkills.xlsx
+++ b/GameDesign/Class/Ninja/Documentation/NinjaSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Cyanide" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="5-Kunai" sheetId="5" r:id="rId5"/>
     <sheet name="6-Shuriken" sheetId="6" r:id="rId6"/>
     <sheet name="7-Makibishi" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
-    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
-    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
+    <sheet name="8-Stealth" sheetId="8" r:id="rId8"/>
+    <sheet name="9-Rin-Hyo" sheetId="9" r:id="rId9"/>
+    <sheet name="10-Tatami" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,65 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="82">
-  <si>
-    <t>[[AP: 0 ]]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>[[MP: 0 ]]</t>
   </si>
   <si>
-    <t>[[Range: 0-0 ]]</t>
-  </si>
-  <si>
-    <t>[[Cast in straight line: - ]]</t>
-  </si>
-  <si>
-    <t>[[Modifiable range: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of casts per turn: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of cast per turn per target: - ]]</t>
-  </si>
-  <si>
-    <t>[[Max effect accumulation: - ]]</t>
-  </si>
-  <si>
-    <t>[[Line of sight: - ]]</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Stright line of 1 cell]]</t>
   </si>
   <si>
     <t>Additional Info</t>
   </si>
   <si>
-    <t>[[Damage:  0-0 fire ]]</t>
-  </si>
-  <si>
-    <t>EX: [[Boost taken damage by 10%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>SKILL DESCRIPTION</t>
-  </si>
-  <si>
-    <t>¨¨ ¨¨</t>
-  </si>
-  <si>
-    <t>SKILL NAME</t>
-  </si>
-  <si>
-    <t>Effect name: ''X''.</t>
-  </si>
-  <si>
-    <t>Unbuff ''X'' effect.</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: -  ]]</t>
-  </si>
-  <si>
     <t>Cyanide</t>
   </si>
   <si>
@@ -185,9 +137,6 @@
     <t>[[Number of cast per turn per target: 2 ]]</t>
   </si>
   <si>
-    <t>[[Damage:  50-60 earth ]]</t>
-  </si>
-  <si>
     <t>I stop hiding, let's face me!</t>
   </si>
   <si>
@@ -279,6 +228,75 @@
   </si>
   <si>
     <t>Let see if you're brave enough to follow me around these.</t>
+  </si>
+  <si>
+    <t>Stealth</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 2-3 ]]</t>
+  </si>
+  <si>
+    <t>Teleport the player at the targeted cell.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - 4 adjacent cell of the targeted cell]]</t>
+  </si>
+  <si>
+    <t>Can only use the skill on a cell adjacent of an big obstacle between the player and the targeted cell.</t>
+  </si>
+  <si>
+    <t>[[Damage:  10 air ]] (Affect only enemies)</t>
+  </si>
+  <si>
+    <t>The darkness opens the way for me</t>
+  </si>
+  <si>
+    <t>[[Damage:  60-70 earth ]]</t>
+  </si>
+  <si>
+    <t>Rin-Hyo</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 4 ]]</t>
+  </si>
+  <si>
+    <t>Target: [[All skill cost 1 AP less then usual]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Target: [[All skill cost 1 more AP then usual]] (1 turn) (Next turn)</t>
+  </si>
+  <si>
+    <t>Effect name 1: ''Hyperactive''.</t>
+  </si>
+  <si>
+    <t>Effect name 2: ''Exhausted''</t>
+  </si>
+  <si>
+    <t>I'll get rid of my opponent before they can react.</t>
+  </si>
+  <si>
+    <t>Tatami</t>
+  </si>
+  <si>
+    <t>Effect name: ''Tatami''.</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 3 ]]</t>
+  </si>
+  <si>
+    <t>When take distance damage, decrase ''Tatami'' by 1 lvl and reduct the damage to 0.</t>
+  </si>
+  <si>
+    <t>[[Tatami +3lvl ]] (1 turns)</t>
+  </si>
+  <si>
+    <t>They will be disappointed!</t>
+  </si>
+  <si>
+    <t>My opponent think I'm vulnerable without a shield…</t>
   </si>
 </sst>
 </file>
@@ -350,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -376,11 +394,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -410,6 +443,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,7 +787,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -760,7 +799,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -772,14 +811,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -791,7 +830,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -803,14 +842,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -822,7 +861,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -834,7 +873,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -852,7 +891,7 @@
     <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -864,14 +903,14 @@
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -888,10 +927,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +950,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -923,14 +962,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -942,21 +981,21 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -968,134 +1007,94 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1128,7 +1127,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1140,7 +1139,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1152,21 +1151,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1178,7 +1177,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1190,14 +1189,14 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1209,7 +1208,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1221,7 +1220,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1239,7 +1238,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1251,14 +1250,14 @@
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="10" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1298,7 +1297,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1310,7 +1309,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1322,21 +1321,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1348,7 +1347,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1360,14 +1359,14 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1379,7 +1378,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1391,14 +1390,14 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1416,7 +1415,7 @@
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1428,7 +1427,7 @@
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="10" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1448,7 +1447,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1467,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1480,7 +1479,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1492,14 +1491,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1511,7 +1510,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1523,14 +1522,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1542,7 +1541,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1554,14 +1553,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1579,7 +1578,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1629,7 +1628,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1641,14 +1640,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1660,21 +1659,21 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1686,21 +1685,21 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1712,14 +1711,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1731,7 +1730,7 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1743,14 +1742,14 @@
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1768,7 +1767,7 @@
     <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -1818,7 +1817,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1830,14 +1829,14 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="9" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1849,14 +1848,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1868,21 +1867,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1894,14 +1893,14 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1913,7 +1912,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1925,28 +1924,28 @@
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1964,7 +1963,7 @@
     <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
       <c r="C27" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1976,7 +1975,7 @@
     <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
       <c r="C29" s="10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -1995,7 +1994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2016,7 +2015,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2028,7 +2027,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2040,14 +2039,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2059,21 +2058,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2085,7 +2084,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2097,7 +2096,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2109,21 +2108,21 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2141,7 +2140,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2153,14 +2152,14 @@
     <row r="26" spans="2:4" ht="98.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="13" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="12" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -2177,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,7 +2199,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2212,179 +2211,139 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="14" t="s">
+        <v>70</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2394,10 +2353,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,7 +2376,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2429,66 +2388,64 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2500,108 +2457,70 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>